<commit_message>
Sistemata la visualizzazione dell'ora dinamica , PROVA A VEDERE LA LIBRERIA OPEN XML INSTED OF SHEETLIGHT
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R9692f5f6e7784300"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rc44751c3b0a4427c"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3267,22 +3267,22 @@
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>2250</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>2250</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>2250</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>2250</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>2250</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>2250</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3340,7 +3340,7 @@
     <x:mergeCell ref="MN1:MT1"/>
     <x:mergeCell ref="MU1:NB1"/>
   </x:mergeCells>
-  <x:conditionalFormatting sqref="B4:H41">
+  <x:conditionalFormatting sqref="B4:H4">
     <x:cfRule type="colorScale" priority="6">
       <x:colorScale>
         <x:cfvo type="min" val="0"/>
@@ -3352,7 +3352,7 @@
       </x:colorScale>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H41">
+  <x:conditionalFormatting sqref="B4:H4">
     <x:cfRule type="colorScale" priority="5">
       <x:colorScale>
         <x:cfvo type="min" val="0"/>
@@ -3364,7 +3364,7 @@
       </x:colorScale>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H41">
+  <x:conditionalFormatting sqref="B4:H4">
     <x:cfRule type="colorScale" priority="4">
       <x:colorScale>
         <x:cfvo type="min" val="0"/>
@@ -3376,7 +3376,7 @@
       </x:colorScale>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H41">
+  <x:conditionalFormatting sqref="B4:H4">
     <x:cfRule type="colorScale" priority="3">
       <x:colorScale>
         <x:cfvo type="min" val="0"/>
@@ -3388,7 +3388,7 @@
       </x:colorScale>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H41">
+  <x:conditionalFormatting sqref="B4:H4">
     <x:cfRule type="colorScale" priority="2">
       <x:colorScale>
         <x:cfvo type="min" val="0"/>
@@ -3400,7 +3400,7 @@
       </x:colorScale>
     </x:cfRule>
   </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H41">
+  <x:conditionalFormatting sqref="B4:H4">
     <x:cfRule type="colorScale" priority="1">
       <x:colorScale>
         <x:cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
finalmente riesco a prendere il valore delle celle
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R0bd0d1b1427e40f5"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R763c42ec2e0e41b2"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -173,9 +173,6 @@
     <x:t xml:space="preserve"> </x:t>
   </x:si>
   <x:si>
-    <x:t>08/04/2019 00:00:00</x:t>
-  </x:si>
-  <x:si>
     <x:t>31/12/2018</x:t>
   </x:si>
   <x:si>
@@ -1272,6 +1269,9 @@
   </x:si>
   <x:si>
     <x:t>31/12/2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09/04/2019 00:00:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1690,7 +1690,7 @@
 
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:NB4"/>
+  <x:dimension ref="A1:NB3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -2173,1124 +2173,1104 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="B2" s="5" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="C2" s="3" t="s">
+      <x:c r="D2" s="3" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="D2" s="3" t="s">
+      <x:c r="E2" s="3" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="E2" s="3" t="s">
+      <x:c r="F2" s="3" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="F2" s="3" t="s">
+      <x:c r="G2" s="3" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="G2" s="3" t="s">
+      <x:c r="H2" s="7" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="H2" s="7" t="s">
+      <x:c r="I2" s="3" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="I2" s="3" t="s">
+      <x:c r="J2" s="3" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="J2" s="3" t="s">
+      <x:c r="K2" s="3" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="K2" s="3" t="s">
+      <x:c r="L2" s="3" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="L2" s="3" t="s">
+      <x:c r="M2" s="3" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="M2" s="3" t="s">
+      <x:c r="N2" s="3" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="N2" s="3" t="s">
+      <x:c r="O2" s="7" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="O2" s="7" t="s">
+      <x:c r="P2" s="3" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="P2" s="3" t="s">
+      <x:c r="Q2" s="3" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="Q2" s="3" t="s">
+      <x:c r="R2" s="3" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="R2" s="3" t="s">
+      <x:c r="S2" s="3" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="S2" s="3" t="s">
+      <x:c r="T2" s="3" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="T2" s="3" t="s">
+      <x:c r="U2" s="3" t="s">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="U2" s="3" t="s">
+      <x:c r="V2" s="7" t="s">
         <x:v>74</x:v>
       </x:c>
-      <x:c r="V2" s="7" t="s">
+      <x:c r="W2" s="3" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="W2" s="3" t="s">
+      <x:c r="X2" s="3" t="s">
         <x:v>76</x:v>
       </x:c>
-      <x:c r="X2" s="3" t="s">
+      <x:c r="Y2" s="3" t="s">
         <x:v>77</x:v>
       </x:c>
-      <x:c r="Y2" s="3" t="s">
+      <x:c r="Z2" s="3" t="s">
         <x:v>78</x:v>
       </x:c>
-      <x:c r="Z2" s="3" t="s">
+      <x:c r="AA2" s="3" t="s">
         <x:v>79</x:v>
       </x:c>
-      <x:c r="AA2" s="3" t="s">
+      <x:c r="AB2" s="3" t="s">
         <x:v>80</x:v>
       </x:c>
-      <x:c r="AB2" s="3" t="s">
+      <x:c r="AC2" s="7" t="s">
         <x:v>81</x:v>
       </x:c>
-      <x:c r="AC2" s="7" t="s">
+      <x:c r="AD2" s="3" t="s">
         <x:v>82</x:v>
       </x:c>
-      <x:c r="AD2" s="3" t="s">
+      <x:c r="AE2" s="3" t="s">
         <x:v>83</x:v>
       </x:c>
-      <x:c r="AE2" s="3" t="s">
+      <x:c r="AF2" s="3" t="s">
         <x:v>84</x:v>
       </x:c>
-      <x:c r="AF2" s="3" t="s">
+      <x:c r="AG2" s="3" t="s">
         <x:v>85</x:v>
       </x:c>
-      <x:c r="AG2" s="3" t="s">
+      <x:c r="AH2" s="3" t="s">
         <x:v>86</x:v>
       </x:c>
-      <x:c r="AH2" s="3" t="s">
+      <x:c r="AI2" s="3" t="s">
         <x:v>87</x:v>
       </x:c>
-      <x:c r="AI2" s="3" t="s">
+      <x:c r="AJ2" s="7" t="s">
         <x:v>88</x:v>
       </x:c>
-      <x:c r="AJ2" s="7" t="s">
+      <x:c r="AK2" s="3" t="s">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="AK2" s="3" t="s">
+      <x:c r="AL2" s="3" t="s">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="AL2" s="3" t="s">
+      <x:c r="AM2" s="3" t="s">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="AM2" s="3" t="s">
+      <x:c r="AN2" s="3" t="s">
         <x:v>92</x:v>
       </x:c>
-      <x:c r="AN2" s="3" t="s">
+      <x:c r="AO2" s="3" t="s">
         <x:v>93</x:v>
       </x:c>
-      <x:c r="AO2" s="3" t="s">
+      <x:c r="AP2" s="3" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="AP2" s="3" t="s">
+      <x:c r="AQ2" s="7" t="s">
         <x:v>95</x:v>
       </x:c>
-      <x:c r="AQ2" s="7" t="s">
+      <x:c r="AR2" s="3" t="s">
         <x:v>96</x:v>
       </x:c>
-      <x:c r="AR2" s="3" t="s">
+      <x:c r="AS2" s="3" t="s">
         <x:v>97</x:v>
       </x:c>
-      <x:c r="AS2" s="3" t="s">
+      <x:c r="AT2" s="3" t="s">
         <x:v>98</x:v>
       </x:c>
-      <x:c r="AT2" s="3" t="s">
+      <x:c r="AU2" s="3" t="s">
         <x:v>99</x:v>
       </x:c>
-      <x:c r="AU2" s="3" t="s">
+      <x:c r="AV2" s="3" t="s">
         <x:v>100</x:v>
       </x:c>
-      <x:c r="AV2" s="3" t="s">
+      <x:c r="AW2" s="3" t="s">
         <x:v>101</x:v>
       </x:c>
-      <x:c r="AW2" s="3" t="s">
+      <x:c r="AX2" s="7" t="s">
         <x:v>102</x:v>
       </x:c>
-      <x:c r="AX2" s="7" t="s">
+      <x:c r="AY2" s="3" t="s">
         <x:v>103</x:v>
       </x:c>
-      <x:c r="AY2" s="3" t="s">
+      <x:c r="AZ2" s="3" t="s">
         <x:v>104</x:v>
       </x:c>
-      <x:c r="AZ2" s="3" t="s">
+      <x:c r="BA2" s="3" t="s">
         <x:v>105</x:v>
       </x:c>
-      <x:c r="BA2" s="3" t="s">
+      <x:c r="BB2" s="3" t="s">
         <x:v>106</x:v>
       </x:c>
-      <x:c r="BB2" s="3" t="s">
+      <x:c r="BC2" s="3" t="s">
         <x:v>107</x:v>
       </x:c>
-      <x:c r="BC2" s="3" t="s">
+      <x:c r="BD2" s="3" t="s">
         <x:v>108</x:v>
       </x:c>
-      <x:c r="BD2" s="3" t="s">
+      <x:c r="BE2" s="7" t="s">
         <x:v>109</x:v>
       </x:c>
-      <x:c r="BE2" s="7" t="s">
+      <x:c r="BF2" s="3" t="s">
         <x:v>110</x:v>
       </x:c>
-      <x:c r="BF2" s="3" t="s">
+      <x:c r="BG2" s="3" t="s">
         <x:v>111</x:v>
       </x:c>
-      <x:c r="BG2" s="3" t="s">
+      <x:c r="BH2" s="3" t="s">
         <x:v>112</x:v>
       </x:c>
-      <x:c r="BH2" s="3" t="s">
+      <x:c r="BI2" s="3" t="s">
         <x:v>113</x:v>
       </x:c>
-      <x:c r="BI2" s="3" t="s">
+      <x:c r="BJ2" s="3" t="s">
         <x:v>114</x:v>
       </x:c>
-      <x:c r="BJ2" s="3" t="s">
+      <x:c r="BK2" s="3" t="s">
         <x:v>115</x:v>
       </x:c>
-      <x:c r="BK2" s="3" t="s">
+      <x:c r="BL2" s="7" t="s">
         <x:v>116</x:v>
       </x:c>
-      <x:c r="BL2" s="7" t="s">
+      <x:c r="BM2" s="3" t="s">
         <x:v>117</x:v>
       </x:c>
-      <x:c r="BM2" s="3" t="s">
+      <x:c r="BN2" s="3" t="s">
         <x:v>118</x:v>
       </x:c>
-      <x:c r="BN2" s="3" t="s">
+      <x:c r="BO2" s="3" t="s">
         <x:v>119</x:v>
       </x:c>
-      <x:c r="BO2" s="3" t="s">
+      <x:c r="BP2" s="3" t="s">
         <x:v>120</x:v>
       </x:c>
-      <x:c r="BP2" s="3" t="s">
+      <x:c r="BQ2" s="3" t="s">
         <x:v>121</x:v>
       </x:c>
-      <x:c r="BQ2" s="3" t="s">
+      <x:c r="BR2" s="3" t="s">
         <x:v>122</x:v>
       </x:c>
-      <x:c r="BR2" s="3" t="s">
+      <x:c r="BS2" s="7" t="s">
         <x:v>123</x:v>
       </x:c>
-      <x:c r="BS2" s="7" t="s">
+      <x:c r="BT2" s="3" t="s">
         <x:v>124</x:v>
       </x:c>
-      <x:c r="BT2" s="3" t="s">
+      <x:c r="BU2" s="3" t="s">
         <x:v>125</x:v>
       </x:c>
-      <x:c r="BU2" s="3" t="s">
+      <x:c r="BV2" s="3" t="s">
         <x:v>126</x:v>
       </x:c>
-      <x:c r="BV2" s="3" t="s">
+      <x:c r="BW2" s="3" t="s">
         <x:v>127</x:v>
       </x:c>
-      <x:c r="BW2" s="3" t="s">
+      <x:c r="BX2" s="3" t="s">
         <x:v>128</x:v>
       </x:c>
-      <x:c r="BX2" s="3" t="s">
+      <x:c r="BY2" s="3" t="s">
         <x:v>129</x:v>
       </x:c>
-      <x:c r="BY2" s="3" t="s">
+      <x:c r="BZ2" s="7" t="s">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="BZ2" s="7" t="s">
+      <x:c r="CA2" s="3" t="s">
         <x:v>131</x:v>
       </x:c>
-      <x:c r="CA2" s="3" t="s">
+      <x:c r="CB2" s="3" t="s">
         <x:v>132</x:v>
       </x:c>
-      <x:c r="CB2" s="3" t="s">
+      <x:c r="CC2" s="3" t="s">
         <x:v>133</x:v>
       </x:c>
-      <x:c r="CC2" s="3" t="s">
+      <x:c r="CD2" s="3" t="s">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="CD2" s="3" t="s">
+      <x:c r="CE2" s="3" t="s">
         <x:v>135</x:v>
       </x:c>
-      <x:c r="CE2" s="3" t="s">
+      <x:c r="CF2" s="3" t="s">
         <x:v>136</x:v>
       </x:c>
-      <x:c r="CF2" s="3" t="s">
+      <x:c r="CG2" s="7" t="s">
         <x:v>137</x:v>
       </x:c>
-      <x:c r="CG2" s="7" t="s">
+      <x:c r="CH2" s="3" t="s">
         <x:v>138</x:v>
       </x:c>
-      <x:c r="CH2" s="3" t="s">
+      <x:c r="CI2" s="3" t="s">
         <x:v>139</x:v>
       </x:c>
-      <x:c r="CI2" s="3" t="s">
+      <x:c r="CJ2" s="3" t="s">
         <x:v>140</x:v>
       </x:c>
-      <x:c r="CJ2" s="3" t="s">
+      <x:c r="CK2" s="3" t="s">
         <x:v>141</x:v>
       </x:c>
-      <x:c r="CK2" s="3" t="s">
+      <x:c r="CL2" s="3" t="s">
         <x:v>142</x:v>
       </x:c>
-      <x:c r="CL2" s="3" t="s">
+      <x:c r="CM2" s="3" t="s">
         <x:v>143</x:v>
       </x:c>
-      <x:c r="CM2" s="3" t="s">
+      <x:c r="CN2" s="7" t="s">
         <x:v>144</x:v>
       </x:c>
-      <x:c r="CN2" s="7" t="s">
+      <x:c r="CO2" s="3" t="s">
         <x:v>145</x:v>
       </x:c>
-      <x:c r="CO2" s="3" t="s">
+      <x:c r="CP2" s="3" t="s">
         <x:v>146</x:v>
       </x:c>
-      <x:c r="CP2" s="3" t="s">
+      <x:c r="CQ2" s="3" t="s">
         <x:v>147</x:v>
       </x:c>
-      <x:c r="CQ2" s="3" t="s">
+      <x:c r="CR2" s="3" t="s">
         <x:v>148</x:v>
       </x:c>
-      <x:c r="CR2" s="3" t="s">
+      <x:c r="CS2" s="3" t="s">
         <x:v>149</x:v>
       </x:c>
-      <x:c r="CS2" s="3" t="s">
+      <x:c r="CT2" s="3" t="s">
         <x:v>150</x:v>
       </x:c>
-      <x:c r="CT2" s="3" t="s">
+      <x:c r="CU2" s="7" t="s">
         <x:v>151</x:v>
       </x:c>
-      <x:c r="CU2" s="7" t="s">
+      <x:c r="CV2" s="3" t="s">
         <x:v>152</x:v>
       </x:c>
-      <x:c r="CV2" s="3" t="s">
+      <x:c r="CW2" s="3" t="s">
         <x:v>153</x:v>
       </x:c>
-      <x:c r="CW2" s="3" t="s">
+      <x:c r="CX2" s="3" t="s">
         <x:v>154</x:v>
       </x:c>
-      <x:c r="CX2" s="3" t="s">
+      <x:c r="CY2" s="3" t="s">
         <x:v>155</x:v>
       </x:c>
-      <x:c r="CY2" s="3" t="s">
+      <x:c r="CZ2" s="3" t="s">
         <x:v>156</x:v>
       </x:c>
-      <x:c r="CZ2" s="3" t="s">
+      <x:c r="DA2" s="3" t="s">
         <x:v>157</x:v>
       </x:c>
-      <x:c r="DA2" s="3" t="s">
+      <x:c r="DB2" s="7" t="s">
         <x:v>158</x:v>
       </x:c>
-      <x:c r="DB2" s="7" t="s">
+      <x:c r="DC2" s="3" t="s">
         <x:v>159</x:v>
       </x:c>
-      <x:c r="DC2" s="3" t="s">
+      <x:c r="DD2" s="3" t="s">
         <x:v>160</x:v>
       </x:c>
-      <x:c r="DD2" s="3" t="s">
+      <x:c r="DE2" s="3" t="s">
         <x:v>161</x:v>
       </x:c>
-      <x:c r="DE2" s="3" t="s">
+      <x:c r="DF2" s="3" t="s">
         <x:v>162</x:v>
       </x:c>
-      <x:c r="DF2" s="3" t="s">
+      <x:c r="DG2" s="3" t="s">
         <x:v>163</x:v>
       </x:c>
-      <x:c r="DG2" s="3" t="s">
+      <x:c r="DH2" s="3" t="s">
         <x:v>164</x:v>
       </x:c>
-      <x:c r="DH2" s="3" t="s">
+      <x:c r="DI2" s="7" t="s">
         <x:v>165</x:v>
       </x:c>
-      <x:c r="DI2" s="7" t="s">
+      <x:c r="DJ2" s="3" t="s">
         <x:v>166</x:v>
       </x:c>
-      <x:c r="DJ2" s="3" t="s">
+      <x:c r="DK2" s="3" t="s">
         <x:v>167</x:v>
       </x:c>
-      <x:c r="DK2" s="3" t="s">
+      <x:c r="DL2" s="3" t="s">
         <x:v>168</x:v>
       </x:c>
-      <x:c r="DL2" s="3" t="s">
+      <x:c r="DM2" s="3" t="s">
         <x:v>169</x:v>
       </x:c>
-      <x:c r="DM2" s="3" t="s">
+      <x:c r="DN2" s="3" t="s">
         <x:v>170</x:v>
       </x:c>
-      <x:c r="DN2" s="3" t="s">
+      <x:c r="DO2" s="3" t="s">
         <x:v>171</x:v>
       </x:c>
-      <x:c r="DO2" s="3" t="s">
+      <x:c r="DP2" s="7" t="s">
         <x:v>172</x:v>
       </x:c>
-      <x:c r="DP2" s="7" t="s">
+      <x:c r="DQ2" s="5" t="s">
         <x:v>173</x:v>
       </x:c>
-      <x:c r="DQ2" s="5" t="s">
+      <x:c r="DR2" s="3" t="s">
         <x:v>174</x:v>
       </x:c>
-      <x:c r="DR2" s="3" t="s">
+      <x:c r="DS2" s="3" t="s">
         <x:v>175</x:v>
       </x:c>
-      <x:c r="DS2" s="3" t="s">
+      <x:c r="DT2" s="3" t="s">
         <x:v>176</x:v>
       </x:c>
-      <x:c r="DT2" s="3" t="s">
+      <x:c r="DU2" s="3" t="s">
         <x:v>177</x:v>
       </x:c>
-      <x:c r="DU2" s="3" t="s">
+      <x:c r="DV2" s="3" t="s">
         <x:v>178</x:v>
       </x:c>
-      <x:c r="DV2" s="3" t="s">
+      <x:c r="DW2" s="3" t="s">
         <x:v>179</x:v>
       </x:c>
-      <x:c r="DW2" s="3" t="s">
+      <x:c r="DX2" s="5" t="s">
         <x:v>180</x:v>
       </x:c>
-      <x:c r="DX2" s="5" t="s">
+      <x:c r="DY2" s="3" t="s">
         <x:v>181</x:v>
       </x:c>
-      <x:c r="DY2" s="3" t="s">
+      <x:c r="DZ2" s="3" t="s">
         <x:v>182</x:v>
       </x:c>
-      <x:c r="DZ2" s="3" t="s">
+      <x:c r="EA2" s="3" t="s">
         <x:v>183</x:v>
       </x:c>
-      <x:c r="EA2" s="3" t="s">
+      <x:c r="EB2" s="3" t="s">
         <x:v>184</x:v>
       </x:c>
-      <x:c r="EB2" s="3" t="s">
+      <x:c r="EC2" s="3" t="s">
         <x:v>185</x:v>
       </x:c>
-      <x:c r="EC2" s="3" t="s">
+      <x:c r="ED2" s="3" t="s">
         <x:v>186</x:v>
       </x:c>
-      <x:c r="ED2" s="3" t="s">
+      <x:c r="EE2" s="5" t="s">
         <x:v>187</x:v>
       </x:c>
-      <x:c r="EE2" s="5" t="s">
+      <x:c r="EF2" s="3" t="s">
         <x:v>188</x:v>
       </x:c>
-      <x:c r="EF2" s="3" t="s">
+      <x:c r="EG2" s="3" t="s">
         <x:v>189</x:v>
       </x:c>
-      <x:c r="EG2" s="3" t="s">
+      <x:c r="EH2" s="3" t="s">
         <x:v>190</x:v>
       </x:c>
-      <x:c r="EH2" s="3" t="s">
+      <x:c r="EI2" s="3" t="s">
         <x:v>191</x:v>
       </x:c>
-      <x:c r="EI2" s="3" t="s">
+      <x:c r="EJ2" s="3" t="s">
         <x:v>192</x:v>
       </x:c>
-      <x:c r="EJ2" s="3" t="s">
+      <x:c r="EK2" s="3" t="s">
         <x:v>193</x:v>
       </x:c>
-      <x:c r="EK2" s="3" t="s">
+      <x:c r="EL2" s="5" t="s">
         <x:v>194</x:v>
       </x:c>
-      <x:c r="EL2" s="5" t="s">
+      <x:c r="EM2" s="3" t="s">
         <x:v>195</x:v>
       </x:c>
-      <x:c r="EM2" s="3" t="s">
+      <x:c r="EN2" s="3" t="s">
         <x:v>196</x:v>
       </x:c>
-      <x:c r="EN2" s="3" t="s">
+      <x:c r="EO2" s="3" t="s">
         <x:v>197</x:v>
       </x:c>
-      <x:c r="EO2" s="3" t="s">
+      <x:c r="EP2" s="3" t="s">
         <x:v>198</x:v>
       </x:c>
-      <x:c r="EP2" s="3" t="s">
+      <x:c r="EQ2" s="3" t="s">
         <x:v>199</x:v>
       </x:c>
-      <x:c r="EQ2" s="3" t="s">
+      <x:c r="ER2" s="3" t="s">
         <x:v>200</x:v>
       </x:c>
-      <x:c r="ER2" s="3" t="s">
+      <x:c r="ES2" s="5" t="s">
         <x:v>201</x:v>
       </x:c>
-      <x:c r="ES2" s="5" t="s">
+      <x:c r="ET2" s="3" t="s">
         <x:v>202</x:v>
       </x:c>
-      <x:c r="ET2" s="3" t="s">
+      <x:c r="EU2" s="3" t="s">
         <x:v>203</x:v>
       </x:c>
-      <x:c r="EU2" s="3" t="s">
+      <x:c r="EV2" s="3" t="s">
         <x:v>204</x:v>
       </x:c>
-      <x:c r="EV2" s="3" t="s">
+      <x:c r="EW2" s="3" t="s">
         <x:v>205</x:v>
       </x:c>
-      <x:c r="EW2" s="3" t="s">
+      <x:c r="EX2" s="3" t="s">
         <x:v>206</x:v>
       </x:c>
-      <x:c r="EX2" s="3" t="s">
+      <x:c r="EY2" s="3" t="s">
         <x:v>207</x:v>
       </x:c>
-      <x:c r="EY2" s="3" t="s">
+      <x:c r="EZ2" s="5" t="s">
         <x:v>208</x:v>
       </x:c>
-      <x:c r="EZ2" s="5" t="s">
+      <x:c r="FA2" s="3" t="s">
         <x:v>209</x:v>
       </x:c>
-      <x:c r="FA2" s="3" t="s">
+      <x:c r="FB2" s="3" t="s">
         <x:v>210</x:v>
       </x:c>
-      <x:c r="FB2" s="3" t="s">
+      <x:c r="FC2" s="3" t="s">
         <x:v>211</x:v>
       </x:c>
-      <x:c r="FC2" s="3" t="s">
+      <x:c r="FD2" s="3" t="s">
         <x:v>212</x:v>
       </x:c>
-      <x:c r="FD2" s="3" t="s">
+      <x:c r="FE2" s="3" t="s">
         <x:v>213</x:v>
       </x:c>
-      <x:c r="FE2" s="3" t="s">
+      <x:c r="FF2" s="3" t="s">
         <x:v>214</x:v>
       </x:c>
-      <x:c r="FF2" s="3" t="s">
+      <x:c r="FG2" s="5" t="s">
         <x:v>215</x:v>
       </x:c>
-      <x:c r="FG2" s="5" t="s">
+      <x:c r="FH2" s="3" t="s">
         <x:v>216</x:v>
       </x:c>
-      <x:c r="FH2" s="3" t="s">
+      <x:c r="FI2" s="3" t="s">
         <x:v>217</x:v>
       </x:c>
-      <x:c r="FI2" s="3" t="s">
+      <x:c r="FJ2" s="3" t="s">
         <x:v>218</x:v>
       </x:c>
-      <x:c r="FJ2" s="3" t="s">
+      <x:c r="FK2" s="3" t="s">
         <x:v>219</x:v>
       </x:c>
-      <x:c r="FK2" s="3" t="s">
+      <x:c r="FL2" s="3" t="s">
         <x:v>220</x:v>
       </x:c>
-      <x:c r="FL2" s="3" t="s">
+      <x:c r="FM2" s="3" t="s">
         <x:v>221</x:v>
       </x:c>
-      <x:c r="FM2" s="3" t="s">
+      <x:c r="FN2" s="5" t="s">
         <x:v>222</x:v>
       </x:c>
-      <x:c r="FN2" s="5" t="s">
+      <x:c r="FO2" s="3" t="s">
         <x:v>223</x:v>
       </x:c>
-      <x:c r="FO2" s="3" t="s">
+      <x:c r="FP2" s="3" t="s">
         <x:v>224</x:v>
       </x:c>
-      <x:c r="FP2" s="3" t="s">
+      <x:c r="FQ2" s="3" t="s">
         <x:v>225</x:v>
       </x:c>
-      <x:c r="FQ2" s="3" t="s">
+      <x:c r="FR2" s="3" t="s">
         <x:v>226</x:v>
       </x:c>
-      <x:c r="FR2" s="3" t="s">
+      <x:c r="FS2" s="3" t="s">
         <x:v>227</x:v>
       </x:c>
-      <x:c r="FS2" s="3" t="s">
+      <x:c r="FT2" s="3" t="s">
         <x:v>228</x:v>
       </x:c>
-      <x:c r="FT2" s="3" t="s">
+      <x:c r="FU2" s="5" t="s">
         <x:v>229</x:v>
       </x:c>
-      <x:c r="FU2" s="5" t="s">
+      <x:c r="FV2" s="3" t="s">
         <x:v>230</x:v>
       </x:c>
-      <x:c r="FV2" s="3" t="s">
+      <x:c r="FW2" s="3" t="s">
         <x:v>231</x:v>
       </x:c>
-      <x:c r="FW2" s="3" t="s">
+      <x:c r="FX2" s="3" t="s">
         <x:v>232</x:v>
       </x:c>
-      <x:c r="FX2" s="3" t="s">
+      <x:c r="FY2" s="3" t="s">
         <x:v>233</x:v>
       </x:c>
-      <x:c r="FY2" s="3" t="s">
+      <x:c r="FZ2" s="3" t="s">
         <x:v>234</x:v>
       </x:c>
-      <x:c r="FZ2" s="3" t="s">
+      <x:c r="GA2" s="3" t="s">
         <x:v>235</x:v>
       </x:c>
-      <x:c r="GA2" s="3" t="s">
+      <x:c r="GB2" s="5" t="s">
         <x:v>236</x:v>
       </x:c>
-      <x:c r="GB2" s="5" t="s">
+      <x:c r="GC2" s="3" t="s">
         <x:v>237</x:v>
       </x:c>
-      <x:c r="GC2" s="3" t="s">
+      <x:c r="GD2" s="3" t="s">
         <x:v>238</x:v>
       </x:c>
-      <x:c r="GD2" s="3" t="s">
+      <x:c r="GE2" s="3" t="s">
         <x:v>239</x:v>
       </x:c>
-      <x:c r="GE2" s="3" t="s">
+      <x:c r="GF2" s="3" t="s">
         <x:v>240</x:v>
       </x:c>
-      <x:c r="GF2" s="3" t="s">
+      <x:c r="GG2" s="3" t="s">
         <x:v>241</x:v>
       </x:c>
-      <x:c r="GG2" s="3" t="s">
+      <x:c r="GH2" s="3" t="s">
         <x:v>242</x:v>
       </x:c>
-      <x:c r="GH2" s="3" t="s">
+      <x:c r="GI2" s="5" t="s">
         <x:v>243</x:v>
       </x:c>
-      <x:c r="GI2" s="5" t="s">
+      <x:c r="GJ2" s="3" t="s">
         <x:v>244</x:v>
       </x:c>
-      <x:c r="GJ2" s="3" t="s">
+      <x:c r="GK2" s="3" t="s">
         <x:v>245</x:v>
       </x:c>
-      <x:c r="GK2" s="3" t="s">
+      <x:c r="GL2" s="3" t="s">
         <x:v>246</x:v>
       </x:c>
-      <x:c r="GL2" s="3" t="s">
+      <x:c r="GM2" s="3" t="s">
         <x:v>247</x:v>
       </x:c>
-      <x:c r="GM2" s="3" t="s">
+      <x:c r="GN2" s="3" t="s">
         <x:v>248</x:v>
       </x:c>
-      <x:c r="GN2" s="3" t="s">
+      <x:c r="GO2" s="3" t="s">
         <x:v>249</x:v>
       </x:c>
-      <x:c r="GO2" s="3" t="s">
+      <x:c r="GP2" s="5" t="s">
         <x:v>250</x:v>
       </x:c>
-      <x:c r="GP2" s="5" t="s">
+      <x:c r="GQ2" s="3" t="s">
         <x:v>251</x:v>
       </x:c>
-      <x:c r="GQ2" s="3" t="s">
+      <x:c r="GR2" s="3" t="s">
         <x:v>252</x:v>
       </x:c>
-      <x:c r="GR2" s="3" t="s">
+      <x:c r="GS2" s="3" t="s">
         <x:v>253</x:v>
       </x:c>
-      <x:c r="GS2" s="3" t="s">
+      <x:c r="GT2" s="3" t="s">
         <x:v>254</x:v>
       </x:c>
-      <x:c r="GT2" s="3" t="s">
+      <x:c r="GU2" s="3" t="s">
         <x:v>255</x:v>
       </x:c>
-      <x:c r="GU2" s="3" t="s">
+      <x:c r="GV2" s="3" t="s">
         <x:v>256</x:v>
       </x:c>
-      <x:c r="GV2" s="3" t="s">
+      <x:c r="GW2" s="5" t="s">
         <x:v>257</x:v>
       </x:c>
-      <x:c r="GW2" s="5" t="s">
+      <x:c r="GX2" s="3" t="s">
         <x:v>258</x:v>
       </x:c>
-      <x:c r="GX2" s="3" t="s">
+      <x:c r="GY2" s="3" t="s">
         <x:v>259</x:v>
       </x:c>
-      <x:c r="GY2" s="3" t="s">
+      <x:c r="GZ2" s="3" t="s">
         <x:v>260</x:v>
       </x:c>
-      <x:c r="GZ2" s="3" t="s">
+      <x:c r="HA2" s="3" t="s">
         <x:v>261</x:v>
       </x:c>
-      <x:c r="HA2" s="3" t="s">
+      <x:c r="HB2" s="3" t="s">
         <x:v>262</x:v>
       </x:c>
-      <x:c r="HB2" s="3" t="s">
+      <x:c r="HC2" s="3" t="s">
         <x:v>263</x:v>
       </x:c>
-      <x:c r="HC2" s="3" t="s">
+      <x:c r="HD2" s="5" t="s">
         <x:v>264</x:v>
       </x:c>
-      <x:c r="HD2" s="5" t="s">
+      <x:c r="HE2" s="3" t="s">
         <x:v>265</x:v>
       </x:c>
-      <x:c r="HE2" s="3" t="s">
+      <x:c r="HF2" s="3" t="s">
         <x:v>266</x:v>
       </x:c>
-      <x:c r="HF2" s="3" t="s">
+      <x:c r="HG2" s="3" t="s">
         <x:v>267</x:v>
       </x:c>
-      <x:c r="HG2" s="3" t="s">
+      <x:c r="HH2" s="3" t="s">
         <x:v>268</x:v>
       </x:c>
-      <x:c r="HH2" s="3" t="s">
+      <x:c r="HI2" s="3" t="s">
         <x:v>269</x:v>
       </x:c>
-      <x:c r="HI2" s="3" t="s">
+      <x:c r="HJ2" s="3" t="s">
         <x:v>270</x:v>
       </x:c>
-      <x:c r="HJ2" s="3" t="s">
+      <x:c r="HK2" s="5" t="s">
         <x:v>271</x:v>
       </x:c>
-      <x:c r="HK2" s="5" t="s">
+      <x:c r="HL2" s="3" t="s">
         <x:v>272</x:v>
       </x:c>
-      <x:c r="HL2" s="3" t="s">
+      <x:c r="HM2" s="3" t="s">
         <x:v>273</x:v>
       </x:c>
-      <x:c r="HM2" s="3" t="s">
+      <x:c r="HN2" s="3" t="s">
         <x:v>274</x:v>
       </x:c>
-      <x:c r="HN2" s="3" t="s">
+      <x:c r="HO2" s="3" t="s">
         <x:v>275</x:v>
       </x:c>
-      <x:c r="HO2" s="3" t="s">
+      <x:c r="HP2" s="3" t="s">
         <x:v>276</x:v>
       </x:c>
-      <x:c r="HP2" s="3" t="s">
+      <x:c r="HQ2" s="3" t="s">
         <x:v>277</x:v>
       </x:c>
-      <x:c r="HQ2" s="3" t="s">
+      <x:c r="HR2" s="5" t="s">
         <x:v>278</x:v>
       </x:c>
-      <x:c r="HR2" s="5" t="s">
+      <x:c r="HS2" s="3" t="s">
         <x:v>279</x:v>
       </x:c>
-      <x:c r="HS2" s="3" t="s">
+      <x:c r="HT2" s="3" t="s">
         <x:v>280</x:v>
       </x:c>
-      <x:c r="HT2" s="3" t="s">
+      <x:c r="HU2" s="3" t="s">
         <x:v>281</x:v>
       </x:c>
-      <x:c r="HU2" s="3" t="s">
+      <x:c r="HV2" s="3" t="s">
         <x:v>282</x:v>
       </x:c>
-      <x:c r="HV2" s="3" t="s">
+      <x:c r="HW2" s="3" t="s">
         <x:v>283</x:v>
       </x:c>
-      <x:c r="HW2" s="3" t="s">
+      <x:c r="HX2" s="3" t="s">
         <x:v>284</x:v>
       </x:c>
-      <x:c r="HX2" s="3" t="s">
+      <x:c r="HY2" s="5" t="s">
         <x:v>285</x:v>
       </x:c>
-      <x:c r="HY2" s="5" t="s">
+      <x:c r="HZ2" s="3" t="s">
         <x:v>286</x:v>
       </x:c>
-      <x:c r="HZ2" s="3" t="s">
+      <x:c r="IA2" s="3" t="s">
         <x:v>287</x:v>
       </x:c>
-      <x:c r="IA2" s="3" t="s">
+      <x:c r="IB2" s="3" t="s">
         <x:v>288</x:v>
       </x:c>
-      <x:c r="IB2" s="3" t="s">
+      <x:c r="IC2" s="3" t="s">
         <x:v>289</x:v>
       </x:c>
-      <x:c r="IC2" s="3" t="s">
+      <x:c r="ID2" s="3" t="s">
         <x:v>290</x:v>
       </x:c>
-      <x:c r="ID2" s="3" t="s">
+      <x:c r="IE2" s="3" t="s">
         <x:v>291</x:v>
       </x:c>
-      <x:c r="IE2" s="3" t="s">
+      <x:c r="IF2" s="5" t="s">
         <x:v>292</x:v>
       </x:c>
-      <x:c r="IF2" s="5" t="s">
+      <x:c r="IG2" s="3" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="IG2" s="3" t="s">
+      <x:c r="IH2" s="3" t="s">
         <x:v>294</x:v>
       </x:c>
-      <x:c r="IH2" s="3" t="s">
+      <x:c r="II2" s="3" t="s">
         <x:v>295</x:v>
       </x:c>
-      <x:c r="II2" s="3" t="s">
+      <x:c r="IJ2" s="3" t="s">
         <x:v>296</x:v>
       </x:c>
-      <x:c r="IJ2" s="3" t="s">
+      <x:c r="IK2" s="3" t="s">
         <x:v>297</x:v>
       </x:c>
-      <x:c r="IK2" s="3" t="s">
+      <x:c r="IL2" s="3" t="s">
         <x:v>298</x:v>
       </x:c>
-      <x:c r="IL2" s="3" t="s">
+      <x:c r="IM2" s="5" t="s">
         <x:v>299</x:v>
       </x:c>
-      <x:c r="IM2" s="5" t="s">
+      <x:c r="IN2" s="3" t="s">
         <x:v>300</x:v>
       </x:c>
-      <x:c r="IN2" s="3" t="s">
+      <x:c r="IO2" s="3" t="s">
         <x:v>301</x:v>
       </x:c>
-      <x:c r="IO2" s="3" t="s">
+      <x:c r="IP2" s="3" t="s">
         <x:v>302</x:v>
       </x:c>
-      <x:c r="IP2" s="3" t="s">
+      <x:c r="IQ2" s="3" t="s">
         <x:v>303</x:v>
       </x:c>
-      <x:c r="IQ2" s="3" t="s">
+      <x:c r="IR2" s="3" t="s">
         <x:v>304</x:v>
       </x:c>
-      <x:c r="IR2" s="3" t="s">
+      <x:c r="IS2" s="3" t="s">
         <x:v>305</x:v>
       </x:c>
-      <x:c r="IS2" s="3" t="s">
+      <x:c r="IT2" s="5" t="s">
         <x:v>306</x:v>
       </x:c>
-      <x:c r="IT2" s="5" t="s">
+      <x:c r="IU2" s="3" t="s">
         <x:v>307</x:v>
       </x:c>
-      <x:c r="IU2" s="3" t="s">
+      <x:c r="IV2" s="3" t="s">
         <x:v>308</x:v>
       </x:c>
-      <x:c r="IV2" s="3" t="s">
+      <x:c r="IW2" s="3" t="s">
         <x:v>309</x:v>
       </x:c>
-      <x:c r="IW2" s="3" t="s">
+      <x:c r="IX2" s="3" t="s">
         <x:v>310</x:v>
       </x:c>
-      <x:c r="IX2" s="3" t="s">
+      <x:c r="IY2" s="3" t="s">
         <x:v>311</x:v>
       </x:c>
-      <x:c r="IY2" s="3" t="s">
+      <x:c r="IZ2" s="3" t="s">
         <x:v>312</x:v>
       </x:c>
-      <x:c r="IZ2" s="3" t="s">
+      <x:c r="JA2" s="5" t="s">
         <x:v>313</x:v>
       </x:c>
-      <x:c r="JA2" s="5" t="s">
+      <x:c r="JB2" s="3" t="s">
         <x:v>314</x:v>
       </x:c>
-      <x:c r="JB2" s="3" t="s">
+      <x:c r="JC2" s="3" t="s">
         <x:v>315</x:v>
       </x:c>
-      <x:c r="JC2" s="3" t="s">
+      <x:c r="JD2" s="3" t="s">
         <x:v>316</x:v>
       </x:c>
-      <x:c r="JD2" s="3" t="s">
+      <x:c r="JE2" s="3" t="s">
         <x:v>317</x:v>
       </x:c>
-      <x:c r="JE2" s="3" t="s">
+      <x:c r="JF2" s="3" t="s">
         <x:v>318</x:v>
       </x:c>
-      <x:c r="JF2" s="3" t="s">
+      <x:c r="JG2" s="3" t="s">
         <x:v>319</x:v>
       </x:c>
-      <x:c r="JG2" s="3" t="s">
+      <x:c r="JH2" s="5" t="s">
         <x:v>320</x:v>
       </x:c>
-      <x:c r="JH2" s="5" t="s">
+      <x:c r="JI2" s="3" t="s">
         <x:v>321</x:v>
       </x:c>
-      <x:c r="JI2" s="3" t="s">
+      <x:c r="JJ2" s="3" t="s">
         <x:v>322</x:v>
       </x:c>
-      <x:c r="JJ2" s="3" t="s">
+      <x:c r="JK2" s="3" t="s">
         <x:v>323</x:v>
       </x:c>
-      <x:c r="JK2" s="3" t="s">
+      <x:c r="JL2" s="3" t="s">
         <x:v>324</x:v>
       </x:c>
-      <x:c r="JL2" s="3" t="s">
+      <x:c r="JM2" s="3" t="s">
         <x:v>325</x:v>
       </x:c>
-      <x:c r="JM2" s="3" t="s">
+      <x:c r="JN2" s="3" t="s">
         <x:v>326</x:v>
       </x:c>
-      <x:c r="JN2" s="3" t="s">
+      <x:c r="JO2" s="5" t="s">
         <x:v>327</x:v>
       </x:c>
-      <x:c r="JO2" s="5" t="s">
+      <x:c r="JP2" s="3" t="s">
         <x:v>328</x:v>
       </x:c>
-      <x:c r="JP2" s="3" t="s">
+      <x:c r="JQ2" s="3" t="s">
         <x:v>329</x:v>
       </x:c>
-      <x:c r="JQ2" s="3" t="s">
+      <x:c r="JR2" s="3" t="s">
         <x:v>330</x:v>
       </x:c>
-      <x:c r="JR2" s="3" t="s">
+      <x:c r="JS2" s="3" t="s">
         <x:v>331</x:v>
       </x:c>
-      <x:c r="JS2" s="3" t="s">
+      <x:c r="JT2" s="3" t="s">
         <x:v>332</x:v>
       </x:c>
-      <x:c r="JT2" s="3" t="s">
+      <x:c r="JU2" s="3" t="s">
         <x:v>333</x:v>
       </x:c>
-      <x:c r="JU2" s="3" t="s">
+      <x:c r="JV2" s="5" t="s">
         <x:v>334</x:v>
       </x:c>
-      <x:c r="JV2" s="5" t="s">
+      <x:c r="JW2" s="3" t="s">
         <x:v>335</x:v>
       </x:c>
-      <x:c r="JW2" s="3" t="s">
+      <x:c r="JX2" s="3" t="s">
         <x:v>336</x:v>
       </x:c>
-      <x:c r="JX2" s="3" t="s">
+      <x:c r="JY2" s="3" t="s">
         <x:v>337</x:v>
       </x:c>
-      <x:c r="JY2" s="3" t="s">
+      <x:c r="JZ2" s="3" t="s">
         <x:v>338</x:v>
       </x:c>
-      <x:c r="JZ2" s="3" t="s">
+      <x:c r="KA2" s="3" t="s">
         <x:v>339</x:v>
       </x:c>
-      <x:c r="KA2" s="3" t="s">
+      <x:c r="KB2" s="3" t="s">
         <x:v>340</x:v>
       </x:c>
-      <x:c r="KB2" s="3" t="s">
+      <x:c r="KC2" s="5" t="s">
         <x:v>341</x:v>
       </x:c>
-      <x:c r="KC2" s="5" t="s">
+      <x:c r="KD2" s="3" t="s">
         <x:v>342</x:v>
       </x:c>
-      <x:c r="KD2" s="3" t="s">
+      <x:c r="KE2" s="3" t="s">
         <x:v>343</x:v>
       </x:c>
-      <x:c r="KE2" s="3" t="s">
+      <x:c r="KF2" s="3" t="s">
         <x:v>344</x:v>
       </x:c>
-      <x:c r="KF2" s="3" t="s">
+      <x:c r="KG2" s="3" t="s">
         <x:v>345</x:v>
       </x:c>
-      <x:c r="KG2" s="3" t="s">
+      <x:c r="KH2" s="3" t="s">
         <x:v>346</x:v>
       </x:c>
-      <x:c r="KH2" s="3" t="s">
+      <x:c r="KI2" s="3" t="s">
         <x:v>347</x:v>
       </x:c>
-      <x:c r="KI2" s="3" t="s">
+      <x:c r="KJ2" s="5" t="s">
         <x:v>348</x:v>
       </x:c>
-      <x:c r="KJ2" s="5" t="s">
+      <x:c r="KK2" s="3" t="s">
         <x:v>349</x:v>
       </x:c>
-      <x:c r="KK2" s="3" t="s">
+      <x:c r="KL2" s="3" t="s">
         <x:v>350</x:v>
       </x:c>
-      <x:c r="KL2" s="3" t="s">
+      <x:c r="KM2" s="3" t="s">
         <x:v>351</x:v>
       </x:c>
-      <x:c r="KM2" s="3" t="s">
+      <x:c r="KN2" s="3" t="s">
         <x:v>352</x:v>
       </x:c>
-      <x:c r="KN2" s="3" t="s">
+      <x:c r="KO2" s="3" t="s">
         <x:v>353</x:v>
       </x:c>
-      <x:c r="KO2" s="3" t="s">
+      <x:c r="KP2" s="3" t="s">
         <x:v>354</x:v>
       </x:c>
-      <x:c r="KP2" s="3" t="s">
+      <x:c r="KQ2" s="5" t="s">
         <x:v>355</x:v>
       </x:c>
-      <x:c r="KQ2" s="5" t="s">
+      <x:c r="KR2" s="3" t="s">
         <x:v>356</x:v>
       </x:c>
-      <x:c r="KR2" s="3" t="s">
+      <x:c r="KS2" s="3" t="s">
         <x:v>357</x:v>
       </x:c>
-      <x:c r="KS2" s="3" t="s">
+      <x:c r="KT2" s="3" t="s">
         <x:v>358</x:v>
       </x:c>
-      <x:c r="KT2" s="3" t="s">
+      <x:c r="KU2" s="3" t="s">
         <x:v>359</x:v>
       </x:c>
-      <x:c r="KU2" s="3" t="s">
+      <x:c r="KV2" s="3" t="s">
         <x:v>360</x:v>
       </x:c>
-      <x:c r="KV2" s="3" t="s">
+      <x:c r="KW2" s="3" t="s">
         <x:v>361</x:v>
       </x:c>
-      <x:c r="KW2" s="3" t="s">
+      <x:c r="KX2" s="5" t="s">
         <x:v>362</x:v>
       </x:c>
-      <x:c r="KX2" s="5" t="s">
+      <x:c r="KY2" s="3" t="s">
         <x:v>363</x:v>
       </x:c>
-      <x:c r="KY2" s="3" t="s">
+      <x:c r="KZ2" s="3" t="s">
         <x:v>364</x:v>
       </x:c>
-      <x:c r="KZ2" s="3" t="s">
+      <x:c r="LA2" s="3" t="s">
         <x:v>365</x:v>
       </x:c>
-      <x:c r="LA2" s="3" t="s">
+      <x:c r="LB2" s="3" t="s">
         <x:v>366</x:v>
       </x:c>
-      <x:c r="LB2" s="3" t="s">
+      <x:c r="LC2" s="3" t="s">
         <x:v>367</x:v>
       </x:c>
-      <x:c r="LC2" s="3" t="s">
+      <x:c r="LD2" s="3" t="s">
         <x:v>368</x:v>
       </x:c>
-      <x:c r="LD2" s="3" t="s">
+      <x:c r="LE2" s="5" t="s">
         <x:v>369</x:v>
       </x:c>
-      <x:c r="LE2" s="5" t="s">
+      <x:c r="LF2" s="3" t="s">
         <x:v>370</x:v>
       </x:c>
-      <x:c r="LF2" s="3" t="s">
+      <x:c r="LG2" s="3" t="s">
         <x:v>371</x:v>
       </x:c>
-      <x:c r="LG2" s="3" t="s">
+      <x:c r="LH2" s="3" t="s">
         <x:v>372</x:v>
       </x:c>
-      <x:c r="LH2" s="3" t="s">
+      <x:c r="LI2" s="3" t="s">
         <x:v>373</x:v>
       </x:c>
-      <x:c r="LI2" s="3" t="s">
+      <x:c r="LJ2" s="3" t="s">
         <x:v>374</x:v>
       </x:c>
-      <x:c r="LJ2" s="3" t="s">
+      <x:c r="LK2" s="3" t="s">
         <x:v>375</x:v>
       </x:c>
-      <x:c r="LK2" s="3" t="s">
+      <x:c r="LL2" s="5" t="s">
         <x:v>376</x:v>
       </x:c>
-      <x:c r="LL2" s="5" t="s">
+      <x:c r="LM2" s="3" t="s">
         <x:v>377</x:v>
       </x:c>
-      <x:c r="LM2" s="3" t="s">
+      <x:c r="LN2" s="3" t="s">
         <x:v>378</x:v>
       </x:c>
-      <x:c r="LN2" s="3" t="s">
+      <x:c r="LO2" s="3" t="s">
         <x:v>379</x:v>
       </x:c>
-      <x:c r="LO2" s="3" t="s">
+      <x:c r="LP2" s="3" t="s">
         <x:v>380</x:v>
       </x:c>
-      <x:c r="LP2" s="3" t="s">
+      <x:c r="LQ2" s="3" t="s">
         <x:v>381</x:v>
       </x:c>
-      <x:c r="LQ2" s="3" t="s">
+      <x:c r="LR2" s="3" t="s">
         <x:v>382</x:v>
       </x:c>
-      <x:c r="LR2" s="3" t="s">
+      <x:c r="LS2" s="5" t="s">
         <x:v>383</x:v>
       </x:c>
-      <x:c r="LS2" s="5" t="s">
+      <x:c r="LT2" s="3" t="s">
         <x:v>384</x:v>
       </x:c>
-      <x:c r="LT2" s="3" t="s">
+      <x:c r="LU2" s="3" t="s">
         <x:v>385</x:v>
       </x:c>
-      <x:c r="LU2" s="3" t="s">
+      <x:c r="LV2" s="3" t="s">
         <x:v>386</x:v>
       </x:c>
-      <x:c r="LV2" s="3" t="s">
+      <x:c r="LW2" s="3" t="s">
         <x:v>387</x:v>
       </x:c>
-      <x:c r="LW2" s="3" t="s">
+      <x:c r="LX2" s="3" t="s">
         <x:v>388</x:v>
       </x:c>
-      <x:c r="LX2" s="3" t="s">
+      <x:c r="LY2" s="3" t="s">
         <x:v>389</x:v>
       </x:c>
-      <x:c r="LY2" s="3" t="s">
+      <x:c r="LZ2" s="5" t="s">
         <x:v>390</x:v>
       </x:c>
-      <x:c r="LZ2" s="5" t="s">
+      <x:c r="MA2" s="3" t="s">
         <x:v>391</x:v>
       </x:c>
-      <x:c r="MA2" s="3" t="s">
+      <x:c r="MB2" s="3" t="s">
         <x:v>392</x:v>
       </x:c>
-      <x:c r="MB2" s="3" t="s">
+      <x:c r="MC2" s="3" t="s">
         <x:v>393</x:v>
       </x:c>
-      <x:c r="MC2" s="3" t="s">
+      <x:c r="MD2" s="3" t="s">
         <x:v>394</x:v>
       </x:c>
-      <x:c r="MD2" s="3" t="s">
+      <x:c r="ME2" s="3" t="s">
         <x:v>395</x:v>
       </x:c>
-      <x:c r="ME2" s="3" t="s">
+      <x:c r="MF2" s="3" t="s">
         <x:v>396</x:v>
       </x:c>
-      <x:c r="MF2" s="3" t="s">
+      <x:c r="MG2" s="5" t="s">
         <x:v>397</x:v>
       </x:c>
-      <x:c r="MG2" s="5" t="s">
+      <x:c r="MH2" s="3" t="s">
         <x:v>398</x:v>
       </x:c>
-      <x:c r="MH2" s="3" t="s">
+      <x:c r="MI2" s="3" t="s">
         <x:v>399</x:v>
       </x:c>
-      <x:c r="MI2" s="3" t="s">
+      <x:c r="MJ2" s="3" t="s">
         <x:v>400</x:v>
       </x:c>
-      <x:c r="MJ2" s="3" t="s">
+      <x:c r="MK2" s="3" t="s">
         <x:v>401</x:v>
       </x:c>
-      <x:c r="MK2" s="3" t="s">
+      <x:c r="ML2" s="3" t="s">
         <x:v>402</x:v>
       </x:c>
-      <x:c r="ML2" s="3" t="s">
+      <x:c r="MM2" s="3" t="s">
         <x:v>403</x:v>
       </x:c>
-      <x:c r="MM2" s="3" t="s">
+      <x:c r="MN2" s="5" t="s">
         <x:v>404</x:v>
       </x:c>
-      <x:c r="MN2" s="5" t="s">
+      <x:c r="MO2" s="3" t="s">
         <x:v>405</x:v>
       </x:c>
-      <x:c r="MO2" s="3" t="s">
+      <x:c r="MP2" s="3" t="s">
         <x:v>406</x:v>
       </x:c>
-      <x:c r="MP2" s="3" t="s">
+      <x:c r="MQ2" s="3" t="s">
         <x:v>407</x:v>
       </x:c>
-      <x:c r="MQ2" s="3" t="s">
+      <x:c r="MR2" s="3" t="s">
         <x:v>408</x:v>
       </x:c>
-      <x:c r="MR2" s="3" t="s">
+      <x:c r="MS2" s="3" t="s">
         <x:v>409</x:v>
       </x:c>
-      <x:c r="MS2" s="3" t="s">
+      <x:c r="MT2" s="3" t="s">
         <x:v>410</x:v>
       </x:c>
-      <x:c r="MT2" s="3" t="s">
+      <x:c r="MU2" s="5" t="s">
         <x:v>411</x:v>
       </x:c>
-      <x:c r="MU2" s="5" t="s">
+      <x:c r="MV2" s="3" t="s">
         <x:v>412</x:v>
       </x:c>
-      <x:c r="MV2" s="3" t="s">
+      <x:c r="MW2" s="3" t="s">
         <x:v>413</x:v>
       </x:c>
-      <x:c r="MW2" s="3" t="s">
+      <x:c r="MX2" s="3" t="s">
         <x:v>414</x:v>
       </x:c>
-      <x:c r="MX2" s="3" t="s">
+      <x:c r="MY2" s="3" t="s">
         <x:v>415</x:v>
       </x:c>
-      <x:c r="MY2" s="3" t="s">
+      <x:c r="MZ2" s="3" t="s">
         <x:v>416</x:v>
       </x:c>
-      <x:c r="MZ2" s="3" t="s">
+      <x:c r="NA2" s="3" t="s">
         <x:v>417</x:v>
       </x:c>
-      <x:c r="NA2" s="3" t="s">
+      <x:c r="NB2" s="7" t="s">
         <x:v>418</x:v>
-      </x:c>
-      <x:c r="NB2" s="7" t="s">
-        <x:v>419</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="C3" t="s">
-        <x:v>53</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4">
-      <x:c r="A4">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B4">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C4">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D4">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E4">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="F4">
-        <x:v>7</x:v>
+        <x:v>419</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -3348,77 +3328,5 @@
     <x:mergeCell ref="MN1:MT1"/>
     <x:mergeCell ref="MU1:NB1"/>
   </x:mergeCells>
-  <x:conditionalFormatting sqref="B4:H4">
-    <x:cfRule type="colorScale" priority="6">
-      <x:colorScale>
-        <x:cfvo type="min" val="0"/>
-        <x:cfvo type="percentile" val="35"/>
-        <x:cfvo type="max" val="0"/>
-        <x:color theme="4" tint="0.2"/>
-        <x:color theme="6" tint="-0.1"/>
-        <x:color theme="9" tint="0.5"/>
-      </x:colorScale>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H4">
-    <x:cfRule type="colorScale" priority="5">
-      <x:colorScale>
-        <x:cfvo type="min" val="0"/>
-        <x:cfvo type="percentile" val="35"/>
-        <x:cfvo type="max" val="0"/>
-        <x:color theme="4" tint="0.2"/>
-        <x:color theme="6" tint="-0.1"/>
-        <x:color theme="9" tint="0.5"/>
-      </x:colorScale>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H4">
-    <x:cfRule type="colorScale" priority="4">
-      <x:colorScale>
-        <x:cfvo type="min" val="0"/>
-        <x:cfvo type="percentile" val="35"/>
-        <x:cfvo type="max" val="0"/>
-        <x:color theme="4" tint="0.2"/>
-        <x:color theme="6" tint="-0.1"/>
-        <x:color theme="9" tint="0.5"/>
-      </x:colorScale>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H4">
-    <x:cfRule type="colorScale" priority="3">
-      <x:colorScale>
-        <x:cfvo type="min" val="0"/>
-        <x:cfvo type="percentile" val="35"/>
-        <x:cfvo type="max" val="0"/>
-        <x:color theme="4" tint="0.2"/>
-        <x:color theme="6" tint="-0.1"/>
-        <x:color theme="9" tint="0.5"/>
-      </x:colorScale>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H4">
-    <x:cfRule type="colorScale" priority="2">
-      <x:colorScale>
-        <x:cfvo type="min" val="0"/>
-        <x:cfvo type="percentile" val="35"/>
-        <x:cfvo type="max" val="0"/>
-        <x:color theme="4" tint="0.2"/>
-        <x:color theme="6" tint="-0.1"/>
-        <x:color theme="9" tint="0.5"/>
-      </x:colorScale>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B4:H4">
-    <x:cfRule type="colorScale" priority="1">
-      <x:colorScale>
-        <x:cfvo type="min" val="0"/>
-        <x:cfvo type="percentile" val="35"/>
-        <x:cfvo type="max" val="0"/>
-        <x:color theme="4" tint="0.2"/>
-        <x:color theme="6" tint="-0.1"/>
-        <x:color theme="9" tint="0.5"/>
-      </x:colorScale>
-    </x:cfRule>
-  </x:conditionalFormatting>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Tentativi di risoluzione del mancato scanning delldata odierna
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R763c42ec2e0e41b2"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R326422b2bffb4796"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="420">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="419">
   <x:si>
     <x:t>W 1</x:t>
   </x:si>
@@ -1269,9 +1269,6 @@
   </x:si>
   <x:si>
     <x:t>31/12/2019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09/04/2019 00:00:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3269,8 +3266,8 @@
       </x:c>
     </x:row>
     <x:row r="3">
-      <x:c r="C3" t="s">
-        <x:v>419</x:v>
+      <x:c r="D3" t="s">
+        <x:v>153</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Non funziona il confronto tra i valori presenti in due celle è assurdo, da risolvere
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R326422b2bffb4796"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R05780c284f014883"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="419">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="420">
   <x:si>
     <x:t>W 1</x:t>
   </x:si>
@@ -1269,6 +1269,9 @@
   </x:si>
   <x:si>
     <x:t>31/12/2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11/04/2019 00:00:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1687,7 +1690,7 @@
 
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:NB3"/>
+  <x:dimension ref="A1:NB4"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -3267,7 +3270,12 @@
     </x:row>
     <x:row r="3">
       <x:c r="D3" t="s">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4">
+      <x:c r="F4" t="s">
+        <x:v>419</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
da finire il controllo data tra due celle
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R05780c284f014883"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R00cc54e5f2054053"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="420">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="419">
   <x:si>
     <x:t>W 1</x:t>
   </x:si>
@@ -1269,9 +1269,6 @@
   </x:si>
   <x:si>
     <x:t>31/12/2019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11/04/2019 00:00:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3270,12 +3267,15 @@
     </x:row>
     <x:row r="3">
       <x:c r="D3" t="s">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
+      <x:c r="D4" t="s">
+        <x:v>155</x:v>
+      </x:c>
       <x:c r="F4" t="s">
-        <x:v>419</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Sistemato il check dell adata, adesso non funziona la colorazione delle caselle
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R00cc54e5f2054053"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Ra469764c24834522"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3265,17 +3265,9 @@
         <x:v>418</x:v>
       </x:c>
     </x:row>
-    <x:row r="3">
-      <x:c r="D3" t="s">
-        <x:v>155</x:v>
-      </x:c>
-    </x:row>
     <x:row r="4">
       <x:c r="D4" t="s">
-        <x:v>155</x:v>
-      </x:c>
-      <x:c r="F4" t="s">
-        <x:v>155</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Da finire il data binding delle informazioni da mettere nella sezione della commessa
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Ra469764c24834522"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rfe23b3b389264f2a"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="419">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="420">
   <x:si>
     <x:t>W 1</x:t>
   </x:si>
@@ -1269,13 +1269,16 @@
   </x:si>
   <x:si>
     <x:t>31/12/2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COMMESSA</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="3">
+  <x:fonts count="4">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
@@ -1290,6 +1293,12 @@
     </x:font>
     <x:font>
       <x:color rgb="FF0000FF"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="12"/>
+      <x:color rgb="FF0000FF"/>
+      <x:name val="Gill-Sans"/>
     </x:font>
   </x:fonts>
   <x:fills count="2">
@@ -1374,7 +1383,7 @@
   <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
-  <x:cellXfs count="8">
+  <x:cellXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1392,6 +1401,12 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" textRotation="90" indent="5" justifyLastLine="1" shrinkToFit="1" readingOrder="2"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <x:alignment horizontal="center" indent="5" justifyLastLine="1" shrinkToFit="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" indent="5" justifyLastLine="1" shrinkToFit="1"/>
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
@@ -1692,9 +1707,14 @@
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="22" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1">
-      <x:c r="A1" s="4"/>
+      <x:c r="A1" s="9" t="s">
+        <x:v>419</x:v>
+      </x:c>
       <x:c r="B1" s="6" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -3267,7 +3287,7 @@
     </x:row>
     <x:row r="4">
       <x:c r="D4" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Da continuare, devo prendere i dati dei risultati e provare a printarli, se vengono presi allora provo ad usare il colore
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rfe23b3b389264f2a"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rb25af34c3ed44ce9"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -1296,7 +1296,7 @@
     </x:font>
     <x:font>
       <x:b/>
-      <x:sz val="12"/>
+      <x:sz val="10"/>
       <x:color rgb="FF0000FF"/>
       <x:name val="Gill-Sans"/>
     </x:font>
@@ -1403,10 +1403,10 @@
       <x:alignment horizontal="center" textRotation="90" indent="5" justifyLastLine="1" shrinkToFit="1" readingOrder="2"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <x:alignment horizontal="center" indent="5" justifyLastLine="1" shrinkToFit="1"/>
+      <x:alignment horizontal="center" textRotation="90" indent="5" justifyLastLine="1" shrinkToFit="1" readingOrder="2"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" indent="5" justifyLastLine="1" shrinkToFit="1"/>
+      <x:alignment horizontal="center" textRotation="90" indent="5" justifyLastLine="1" shrinkToFit="1" readingOrder="2"/>
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
@@ -1708,13 +1708,11 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="22" customWidth="1"/>
+    <x:col min="1" max="1" width="25" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1">
-      <x:c r="A1" s="9" t="s">
-        <x:v>419</x:v>
-      </x:c>
+      <x:c r="A1" s="9"/>
       <x:c r="B1" s="6" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -2187,7 +2185,7 @@
     </x:row>
     <x:row r="2">
       <x:c r="A2" s="3" t="s">
-        <x:v>52</x:v>
+        <x:v>419</x:v>
       </x:c>
       <x:c r="B2" s="5" t="s">
         <x:v>54</x:v>
@@ -3287,7 +3285,7 @@
     </x:row>
     <x:row r="4">
       <x:c r="D4" t="s">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Non riesco a trovare una soluzione per il printing nelle celle che si riferiscono ai tempi delle lavorazioni
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R6a77405ec96a4734"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R487c925128044026"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="420">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="421">
   <x:si>
     <x:t>W 1</x:t>
   </x:si>
@@ -1272,6 +1272,9 @@
   </x:si>
   <x:si>
     <x:t>COMMESSA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>imnho</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1702,7 +1705,7 @@
 
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:NB500"/>
+  <x:dimension ref="A1:NB6"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -2184,8 +2187,8 @@
       <x:c r="NB1" s="4"/>
     </x:row>
     <x:row r="2">
-      <x:c r="A2" s="3">
-        <x:v>2</x:v>
+      <x:c r="A2" s="3" t="s">
+        <x:v>419</x:v>
       </x:c>
       <x:c r="B2" s="5" t="s">
         <x:v>54</x:v>
@@ -3283,2497 +3286,14 @@
         <x:v>418</x:v>
       </x:c>
     </x:row>
-    <x:row r="3">
-      <x:c r="A3">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
     <x:row r="4">
-      <x:c r="A4">
-        <x:v>4</x:v>
-      </x:c>
       <x:c r="D4" t="s">
-        <x:v>162</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5">
-      <x:c r="A5">
-        <x:v>5</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
-      <x:c r="A6">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7">
-      <x:c r="A7">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8">
-      <x:c r="A8">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9">
-      <x:c r="A9">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10">
-      <x:c r="A10">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11">
-      <x:c r="A11">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12">
-      <x:c r="A12">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13">
-      <x:c r="A13">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14">
-      <x:c r="A14">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15">
-      <x:c r="A15">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16">
-      <x:c r="A16">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17">
-      <x:c r="A17">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18">
-      <x:c r="A18">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19">
-      <x:c r="A19">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20">
-      <x:c r="A20">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21">
-      <x:c r="A21">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22">
-      <x:c r="A22">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23">
-      <x:c r="A23">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24">
-      <x:c r="A24">
-        <x:v>24</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25">
-      <x:c r="A25">
-        <x:v>25</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26">
-      <x:c r="A26">
-        <x:v>26</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27">
-      <x:c r="A27">
-        <x:v>27</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28">
-      <x:c r="A28">
-        <x:v>28</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29">
-      <x:c r="A29">
-        <x:v>29</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30">
-      <x:c r="A30">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31">
-      <x:c r="A31">
-        <x:v>31</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32">
-      <x:c r="A32">
-        <x:v>32</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33">
-      <x:c r="A33">
-        <x:v>33</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34">
-      <x:c r="A34">
-        <x:v>34</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35">
-      <x:c r="A35">
-        <x:v>35</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36">
-      <x:c r="A36">
-        <x:v>36</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37">
-      <x:c r="A37">
-        <x:v>37</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38">
-      <x:c r="A38">
-        <x:v>38</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39">
-      <x:c r="A39">
-        <x:v>39</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40">
-      <x:c r="A40">
-        <x:v>40</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41">
-      <x:c r="A41">
-        <x:v>41</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42">
-      <x:c r="A42">
-        <x:v>42</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43">
-      <x:c r="A43">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44">
-      <x:c r="A44">
-        <x:v>44</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="45">
-      <x:c r="A45">
-        <x:v>45</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="46">
-      <x:c r="A46">
-        <x:v>46</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="47">
-      <x:c r="A47">
-        <x:v>47</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="48">
-      <x:c r="A48">
-        <x:v>48</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="49">
-      <x:c r="A49">
-        <x:v>49</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="50">
-      <x:c r="A50">
-        <x:v>50</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="51">
-      <x:c r="A51">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="52">
-      <x:c r="A52">
-        <x:v>52</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="53">
-      <x:c r="A53">
-        <x:v>53</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="54">
-      <x:c r="A54">
-        <x:v>54</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="55">
-      <x:c r="A55">
-        <x:v>55</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="56">
-      <x:c r="A56">
-        <x:v>56</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="57">
-      <x:c r="A57">
-        <x:v>57</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="58">
-      <x:c r="A58">
-        <x:v>58</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="59">
-      <x:c r="A59">
-        <x:v>59</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="60">
-      <x:c r="A60">
-        <x:v>60</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="61">
-      <x:c r="A61">
-        <x:v>61</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="62">
-      <x:c r="A62">
-        <x:v>62</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="63">
-      <x:c r="A63">
-        <x:v>63</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="64">
-      <x:c r="A64">
-        <x:v>64</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="65">
-      <x:c r="A65">
-        <x:v>65</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="66">
-      <x:c r="A66">
-        <x:v>66</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="67">
-      <x:c r="A67">
-        <x:v>67</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="68">
-      <x:c r="A68">
-        <x:v>68</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="69">
-      <x:c r="A69">
-        <x:v>69</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="70">
-      <x:c r="A70">
-        <x:v>70</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="71">
-      <x:c r="A71">
-        <x:v>71</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="72">
-      <x:c r="A72">
-        <x:v>72</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="73">
-      <x:c r="A73">
-        <x:v>73</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="74">
-      <x:c r="A74">
-        <x:v>74</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="75">
-      <x:c r="A75">
-        <x:v>75</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="76">
-      <x:c r="A76">
-        <x:v>76</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="77">
-      <x:c r="A77">
-        <x:v>77</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="78">
-      <x:c r="A78">
-        <x:v>78</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="79">
-      <x:c r="A79">
-        <x:v>79</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="80">
-      <x:c r="A80">
-        <x:v>80</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="81">
-      <x:c r="A81">
-        <x:v>81</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="82">
-      <x:c r="A82">
-        <x:v>82</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="83">
-      <x:c r="A83">
-        <x:v>83</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="84">
-      <x:c r="A84">
-        <x:v>84</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="85">
-      <x:c r="A85">
-        <x:v>85</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="86">
-      <x:c r="A86">
-        <x:v>86</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="87">
-      <x:c r="A87">
-        <x:v>87</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="88">
-      <x:c r="A88">
-        <x:v>88</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="89">
-      <x:c r="A89">
-        <x:v>89</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="90">
-      <x:c r="A90">
-        <x:v>90</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="91">
-      <x:c r="A91">
-        <x:v>91</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="92">
-      <x:c r="A92">
-        <x:v>92</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="93">
-      <x:c r="A93">
-        <x:v>93</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="94">
-      <x:c r="A94">
-        <x:v>94</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="95">
-      <x:c r="A95">
-        <x:v>95</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="96">
-      <x:c r="A96">
-        <x:v>96</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="97">
-      <x:c r="A97">
-        <x:v>97</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="98">
-      <x:c r="A98">
-        <x:v>98</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="99">
-      <x:c r="A99">
-        <x:v>99</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="100">
-      <x:c r="A100">
-        <x:v>100</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="101">
-      <x:c r="A101">
-        <x:v>101</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="102">
-      <x:c r="A102">
-        <x:v>102</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="103">
-      <x:c r="A103">
-        <x:v>103</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="104">
-      <x:c r="A104">
-        <x:v>104</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="105">
-      <x:c r="A105">
-        <x:v>105</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="106">
-      <x:c r="A106">
-        <x:v>106</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="107">
-      <x:c r="A107">
-        <x:v>107</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="108">
-      <x:c r="A108">
-        <x:v>108</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="109">
-      <x:c r="A109">
-        <x:v>109</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="110">
-      <x:c r="A110">
-        <x:v>110</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="111">
-      <x:c r="A111">
-        <x:v>111</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="112">
-      <x:c r="A112">
-        <x:v>112</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="113">
-      <x:c r="A113">
-        <x:v>113</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="114">
-      <x:c r="A114">
-        <x:v>114</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="115">
-      <x:c r="A115">
-        <x:v>115</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="116">
-      <x:c r="A116">
-        <x:v>116</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="117">
-      <x:c r="A117">
-        <x:v>117</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="118">
-      <x:c r="A118">
-        <x:v>118</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="119">
-      <x:c r="A119">
-        <x:v>119</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="120">
-      <x:c r="A120">
-        <x:v>120</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="121">
-      <x:c r="A121">
-        <x:v>121</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="122">
-      <x:c r="A122">
-        <x:v>122</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="123">
-      <x:c r="A123">
-        <x:v>123</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="124">
-      <x:c r="A124">
-        <x:v>124</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="125">
-      <x:c r="A125">
-        <x:v>125</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="126">
-      <x:c r="A126">
-        <x:v>126</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="127">
-      <x:c r="A127">
-        <x:v>127</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="128">
-      <x:c r="A128">
-        <x:v>128</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="129">
-      <x:c r="A129">
-        <x:v>129</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="130">
-      <x:c r="A130">
-        <x:v>130</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="131">
-      <x:c r="A131">
-        <x:v>131</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="132">
-      <x:c r="A132">
-        <x:v>132</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="133">
-      <x:c r="A133">
-        <x:v>133</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="134">
-      <x:c r="A134">
-        <x:v>134</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="135">
-      <x:c r="A135">
-        <x:v>135</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="136">
-      <x:c r="A136">
-        <x:v>136</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="137">
-      <x:c r="A137">
-        <x:v>137</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="138">
-      <x:c r="A138">
-        <x:v>138</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="139">
-      <x:c r="A139">
-        <x:v>139</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="140">
-      <x:c r="A140">
-        <x:v>140</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="141">
-      <x:c r="A141">
-        <x:v>141</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="142">
-      <x:c r="A142">
-        <x:v>142</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="143">
-      <x:c r="A143">
-        <x:v>143</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="144">
-      <x:c r="A144">
-        <x:v>144</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="145">
-      <x:c r="A145">
-        <x:v>145</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="146">
-      <x:c r="A146">
-        <x:v>146</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="147">
-      <x:c r="A147">
-        <x:v>147</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="148">
-      <x:c r="A148">
-        <x:v>148</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="149">
-      <x:c r="A149">
-        <x:v>149</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="150">
-      <x:c r="A150">
-        <x:v>150</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="151">
-      <x:c r="A151">
-        <x:v>151</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="152">
-      <x:c r="A152">
-        <x:v>152</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="153">
-      <x:c r="A153">
-        <x:v>153</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="154">
-      <x:c r="A154">
-        <x:v>154</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="155">
-      <x:c r="A155">
-        <x:v>155</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="156">
-      <x:c r="A156">
-        <x:v>156</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="157">
-      <x:c r="A157">
-        <x:v>157</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="158">
-      <x:c r="A158">
-        <x:v>158</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="159">
-      <x:c r="A159">
-        <x:v>159</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="160">
-      <x:c r="A160">
-        <x:v>160</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="161">
-      <x:c r="A161">
-        <x:v>161</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="162">
-      <x:c r="A162">
-        <x:v>162</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="163">
-      <x:c r="A163">
-        <x:v>163</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="164">
-      <x:c r="A164">
-        <x:v>164</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="165">
-      <x:c r="A165">
-        <x:v>165</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="166">
-      <x:c r="A166">
-        <x:v>166</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="167">
-      <x:c r="A167">
-        <x:v>167</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="168">
-      <x:c r="A168">
-        <x:v>168</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="169">
-      <x:c r="A169">
-        <x:v>169</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="170">
-      <x:c r="A170">
-        <x:v>170</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="171">
-      <x:c r="A171">
-        <x:v>171</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="172">
-      <x:c r="A172">
-        <x:v>172</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="173">
-      <x:c r="A173">
-        <x:v>173</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="174">
-      <x:c r="A174">
-        <x:v>174</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="175">
-      <x:c r="A175">
-        <x:v>175</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="176">
-      <x:c r="A176">
-        <x:v>176</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="177">
-      <x:c r="A177">
-        <x:v>177</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="178">
-      <x:c r="A178">
-        <x:v>178</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="179">
-      <x:c r="A179">
-        <x:v>179</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="180">
-      <x:c r="A180">
-        <x:v>180</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="181">
-      <x:c r="A181">
-        <x:v>181</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="182">
-      <x:c r="A182">
-        <x:v>182</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="183">
-      <x:c r="A183">
-        <x:v>183</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="184">
-      <x:c r="A184">
-        <x:v>184</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="185">
-      <x:c r="A185">
-        <x:v>185</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="186">
-      <x:c r="A186">
-        <x:v>186</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="187">
-      <x:c r="A187">
-        <x:v>187</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="188">
-      <x:c r="A188">
-        <x:v>188</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="189">
-      <x:c r="A189">
-        <x:v>189</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="190">
-      <x:c r="A190">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="191">
-      <x:c r="A191">
-        <x:v>191</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="192">
-      <x:c r="A192">
-        <x:v>192</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="193">
-      <x:c r="A193">
-        <x:v>193</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="194">
-      <x:c r="A194">
-        <x:v>194</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="195">
-      <x:c r="A195">
-        <x:v>195</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="196">
-      <x:c r="A196">
-        <x:v>196</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="197">
-      <x:c r="A197">
-        <x:v>197</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="198">
-      <x:c r="A198">
-        <x:v>198</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="199">
-      <x:c r="A199">
-        <x:v>199</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="200">
-      <x:c r="A200">
-        <x:v>200</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="201">
-      <x:c r="A201">
-        <x:v>201</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="202">
-      <x:c r="A202">
-        <x:v>202</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="203">
-      <x:c r="A203">
-        <x:v>203</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="204">
-      <x:c r="A204">
-        <x:v>204</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="205">
-      <x:c r="A205">
-        <x:v>205</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="206">
-      <x:c r="A206">
-        <x:v>206</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="207">
-      <x:c r="A207">
-        <x:v>207</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="208">
-      <x:c r="A208">
-        <x:v>208</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="209">
-      <x:c r="A209">
-        <x:v>209</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="210">
-      <x:c r="A210">
-        <x:v>210</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="211">
-      <x:c r="A211">
-        <x:v>211</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="212">
-      <x:c r="A212">
-        <x:v>212</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="213">
-      <x:c r="A213">
-        <x:v>213</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="214">
-      <x:c r="A214">
-        <x:v>214</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="215">
-      <x:c r="A215">
-        <x:v>215</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="216">
-      <x:c r="A216">
-        <x:v>216</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="217">
-      <x:c r="A217">
-        <x:v>217</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="218">
-      <x:c r="A218">
-        <x:v>218</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="219">
-      <x:c r="A219">
-        <x:v>219</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="220">
-      <x:c r="A220">
-        <x:v>220</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="221">
-      <x:c r="A221">
-        <x:v>221</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="222">
-      <x:c r="A222">
-        <x:v>222</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="223">
-      <x:c r="A223">
-        <x:v>223</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="224">
-      <x:c r="A224">
-        <x:v>224</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="225">
-      <x:c r="A225">
-        <x:v>225</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="226">
-      <x:c r="A226">
-        <x:v>226</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="227">
-      <x:c r="A227">
-        <x:v>227</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="228">
-      <x:c r="A228">
-        <x:v>228</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="229">
-      <x:c r="A229">
-        <x:v>229</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="230">
-      <x:c r="A230">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="231">
-      <x:c r="A231">
-        <x:v>231</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="232">
-      <x:c r="A232">
-        <x:v>232</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="233">
-      <x:c r="A233">
-        <x:v>233</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="234">
-      <x:c r="A234">
-        <x:v>234</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="235">
-      <x:c r="A235">
-        <x:v>235</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="236">
-      <x:c r="A236">
-        <x:v>236</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="237">
-      <x:c r="A237">
-        <x:v>237</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="238">
-      <x:c r="A238">
-        <x:v>238</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="239">
-      <x:c r="A239">
-        <x:v>239</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="240">
-      <x:c r="A240">
-        <x:v>240</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="241">
-      <x:c r="A241">
-        <x:v>241</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="242">
-      <x:c r="A242">
-        <x:v>242</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="243">
-      <x:c r="A243">
-        <x:v>243</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="244">
-      <x:c r="A244">
-        <x:v>244</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="245">
-      <x:c r="A245">
-        <x:v>245</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="246">
-      <x:c r="A246">
-        <x:v>246</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="247">
-      <x:c r="A247">
-        <x:v>247</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="248">
-      <x:c r="A248">
-        <x:v>248</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="249">
-      <x:c r="A249">
-        <x:v>249</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="250">
-      <x:c r="A250">
-        <x:v>250</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="251">
-      <x:c r="A251">
-        <x:v>251</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="252">
-      <x:c r="A252">
-        <x:v>252</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="253">
-      <x:c r="A253">
-        <x:v>253</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="254">
-      <x:c r="A254">
-        <x:v>254</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="255">
-      <x:c r="A255">
-        <x:v>255</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="256">
-      <x:c r="A256">
-        <x:v>256</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="257">
-      <x:c r="A257">
-        <x:v>257</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="258">
-      <x:c r="A258">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="259">
-      <x:c r="A259">
-        <x:v>259</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="260">
-      <x:c r="A260">
-        <x:v>260</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="261">
-      <x:c r="A261">
-        <x:v>261</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="262">
-      <x:c r="A262">
-        <x:v>262</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="263">
-      <x:c r="A263">
-        <x:v>263</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="264">
-      <x:c r="A264">
-        <x:v>264</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="265">
-      <x:c r="A265">
-        <x:v>265</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="266">
-      <x:c r="A266">
-        <x:v>266</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="267">
-      <x:c r="A267">
-        <x:v>267</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="268">
-      <x:c r="A268">
-        <x:v>268</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="269">
-      <x:c r="A269">
-        <x:v>269</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="270">
-      <x:c r="A270">
-        <x:v>270</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="271">
-      <x:c r="A271">
-        <x:v>271</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="272">
-      <x:c r="A272">
-        <x:v>272</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="273">
-      <x:c r="A273">
-        <x:v>273</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="274">
-      <x:c r="A274">
-        <x:v>274</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="275">
-      <x:c r="A275">
-        <x:v>275</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="276">
-      <x:c r="A276">
-        <x:v>276</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="277">
-      <x:c r="A277">
-        <x:v>277</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="278">
-      <x:c r="A278">
-        <x:v>278</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="279">
-      <x:c r="A279">
-        <x:v>279</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="280">
-      <x:c r="A280">
-        <x:v>280</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="281">
-      <x:c r="A281">
-        <x:v>281</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="282">
-      <x:c r="A282">
-        <x:v>282</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="283">
-      <x:c r="A283">
-        <x:v>283</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="284">
-      <x:c r="A284">
-        <x:v>284</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="285">
-      <x:c r="A285">
-        <x:v>285</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="286">
-      <x:c r="A286">
-        <x:v>286</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="287">
-      <x:c r="A287">
-        <x:v>287</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="288">
-      <x:c r="A288">
-        <x:v>288</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="289">
-      <x:c r="A289">
-        <x:v>289</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="290">
-      <x:c r="A290">
-        <x:v>290</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="291">
-      <x:c r="A291">
-        <x:v>291</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="292">
-      <x:c r="A292">
-        <x:v>292</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="293">
-      <x:c r="A293">
-        <x:v>293</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="294">
-      <x:c r="A294">
-        <x:v>294</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="295">
-      <x:c r="A295">
-        <x:v>295</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="296">
-      <x:c r="A296">
-        <x:v>296</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="297">
-      <x:c r="A297">
-        <x:v>297</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="298">
-      <x:c r="A298">
-        <x:v>298</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="299">
-      <x:c r="A299">
-        <x:v>299</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="300">
-      <x:c r="A300">
-        <x:v>300</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="301">
-      <x:c r="A301">
-        <x:v>301</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="302">
-      <x:c r="A302">
-        <x:v>302</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="303">
-      <x:c r="A303">
-        <x:v>303</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="304">
-      <x:c r="A304">
-        <x:v>304</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="305">
-      <x:c r="A305">
-        <x:v>305</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="306">
-      <x:c r="A306">
-        <x:v>306</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="307">
-      <x:c r="A307">
-        <x:v>307</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="308">
-      <x:c r="A308">
-        <x:v>308</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="309">
-      <x:c r="A309">
-        <x:v>309</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="310">
-      <x:c r="A310">
-        <x:v>310</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="311">
-      <x:c r="A311">
-        <x:v>311</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="312">
-      <x:c r="A312">
-        <x:v>312</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="313">
-      <x:c r="A313">
-        <x:v>313</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="314">
-      <x:c r="A314">
-        <x:v>314</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="315">
-      <x:c r="A315">
-        <x:v>315</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="316">
-      <x:c r="A316">
-        <x:v>316</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="317">
-      <x:c r="A317">
-        <x:v>317</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="318">
-      <x:c r="A318">
-        <x:v>318</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="319">
-      <x:c r="A319">
-        <x:v>319</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="320">
-      <x:c r="A320">
-        <x:v>320</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="321">
-      <x:c r="A321">
-        <x:v>321</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="322">
-      <x:c r="A322">
-        <x:v>322</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="323">
-      <x:c r="A323">
-        <x:v>323</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="324">
-      <x:c r="A324">
-        <x:v>324</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="325">
-      <x:c r="A325">
-        <x:v>325</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="326">
-      <x:c r="A326">
-        <x:v>326</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="327">
-      <x:c r="A327">
-        <x:v>327</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="328">
-      <x:c r="A328">
-        <x:v>328</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="329">
-      <x:c r="A329">
-        <x:v>329</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="330">
-      <x:c r="A330">
-        <x:v>330</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="331">
-      <x:c r="A331">
-        <x:v>331</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="332">
-      <x:c r="A332">
-        <x:v>332</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="333">
-      <x:c r="A333">
-        <x:v>333</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="334">
-      <x:c r="A334">
-        <x:v>334</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="335">
-      <x:c r="A335">
-        <x:v>335</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="336">
-      <x:c r="A336">
-        <x:v>336</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="337">
-      <x:c r="A337">
-        <x:v>337</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="338">
-      <x:c r="A338">
-        <x:v>338</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="339">
-      <x:c r="A339">
-        <x:v>339</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="340">
-      <x:c r="A340">
-        <x:v>340</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="341">
-      <x:c r="A341">
-        <x:v>341</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="342">
-      <x:c r="A342">
-        <x:v>342</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="343">
-      <x:c r="A343">
-        <x:v>343</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="344">
-      <x:c r="A344">
-        <x:v>344</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="345">
-      <x:c r="A345">
-        <x:v>345</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="346">
-      <x:c r="A346">
-        <x:v>346</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="347">
-      <x:c r="A347">
-        <x:v>347</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="348">
-      <x:c r="A348">
-        <x:v>348</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="349">
-      <x:c r="A349">
-        <x:v>349</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="350">
-      <x:c r="A350">
-        <x:v>350</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="351">
-      <x:c r="A351">
-        <x:v>351</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="352">
-      <x:c r="A352">
-        <x:v>352</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="353">
-      <x:c r="A353">
-        <x:v>353</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="354">
-      <x:c r="A354">
-        <x:v>354</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="355">
-      <x:c r="A355">
-        <x:v>355</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="356">
-      <x:c r="A356">
-        <x:v>356</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="357">
-      <x:c r="A357">
-        <x:v>357</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="358">
-      <x:c r="A358">
-        <x:v>358</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="359">
-      <x:c r="A359">
-        <x:v>359</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="360">
-      <x:c r="A360">
-        <x:v>360</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="361">
-      <x:c r="A361">
-        <x:v>361</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="362">
-      <x:c r="A362">
-        <x:v>362</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="363">
-      <x:c r="A363">
-        <x:v>363</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="364">
-      <x:c r="A364">
-        <x:v>364</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="365">
-      <x:c r="A365">
-        <x:v>365</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="366">
-      <x:c r="A366">
-        <x:v>366</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="367">
-      <x:c r="A367">
-        <x:v>367</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="368">
-      <x:c r="A368">
-        <x:v>368</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="369">
-      <x:c r="A369">
-        <x:v>369</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="370">
-      <x:c r="A370">
-        <x:v>370</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="371">
-      <x:c r="A371">
-        <x:v>371</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="372">
-      <x:c r="A372">
-        <x:v>372</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="373">
-      <x:c r="A373">
-        <x:v>373</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="374">
-      <x:c r="A374">
-        <x:v>374</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="375">
-      <x:c r="A375">
-        <x:v>375</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="376">
-      <x:c r="A376">
-        <x:v>376</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="377">
-      <x:c r="A377">
-        <x:v>377</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="378">
-      <x:c r="A378">
-        <x:v>378</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="379">
-      <x:c r="A379">
-        <x:v>379</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="380">
-      <x:c r="A380">
-        <x:v>380</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="381">
-      <x:c r="A381">
-        <x:v>381</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="382">
-      <x:c r="A382">
-        <x:v>382</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="383">
-      <x:c r="A383">
-        <x:v>383</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="384">
-      <x:c r="A384">
-        <x:v>384</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="385">
-      <x:c r="A385">
-        <x:v>385</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="386">
-      <x:c r="A386">
-        <x:v>386</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="387">
-      <x:c r="A387">
-        <x:v>387</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="388">
-      <x:c r="A388">
-        <x:v>388</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="389">
-      <x:c r="A389">
-        <x:v>389</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="390">
-      <x:c r="A390">
-        <x:v>390</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="391">
-      <x:c r="A391">
-        <x:v>391</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="392">
-      <x:c r="A392">
-        <x:v>392</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="393">
-      <x:c r="A393">
-        <x:v>393</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="394">
-      <x:c r="A394">
-        <x:v>394</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="395">
-      <x:c r="A395">
-        <x:v>395</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="396">
-      <x:c r="A396">
-        <x:v>396</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="397">
-      <x:c r="A397">
-        <x:v>397</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="398">
-      <x:c r="A398">
-        <x:v>398</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="399">
-      <x:c r="A399">
-        <x:v>399</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="400">
-      <x:c r="A400">
-        <x:v>400</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="401">
-      <x:c r="A401">
-        <x:v>401</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="402">
-      <x:c r="A402">
-        <x:v>402</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="403">
-      <x:c r="A403">
-        <x:v>403</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="404">
-      <x:c r="A404">
-        <x:v>404</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="405">
-      <x:c r="A405">
-        <x:v>405</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="406">
-      <x:c r="A406">
-        <x:v>406</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="407">
-      <x:c r="A407">
-        <x:v>407</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="408">
-      <x:c r="A408">
-        <x:v>408</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="409">
-      <x:c r="A409">
-        <x:v>409</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="410">
-      <x:c r="A410">
-        <x:v>410</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="411">
-      <x:c r="A411">
-        <x:v>411</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="412">
-      <x:c r="A412">
-        <x:v>412</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="413">
-      <x:c r="A413">
-        <x:v>413</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="414">
-      <x:c r="A414">
-        <x:v>414</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="415">
-      <x:c r="A415">
-        <x:v>415</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="416">
-      <x:c r="A416">
-        <x:v>416</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="417">
-      <x:c r="A417">
-        <x:v>417</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="418">
-      <x:c r="A418">
-        <x:v>418</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="419">
-      <x:c r="A419">
-        <x:v>419</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="420">
-      <x:c r="A420">
+      <x:c r="A6" t="s">
         <x:v>420</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="421">
-      <x:c r="A421">
-        <x:v>421</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="422">
-      <x:c r="A422">
-        <x:v>422</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="423">
-      <x:c r="A423">
-        <x:v>423</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="424">
-      <x:c r="A424">
-        <x:v>424</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="425">
-      <x:c r="A425">
-        <x:v>425</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="426">
-      <x:c r="A426">
-        <x:v>426</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="427">
-      <x:c r="A427">
-        <x:v>427</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="428">
-      <x:c r="A428">
-        <x:v>428</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="429">
-      <x:c r="A429">
-        <x:v>429</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="430">
-      <x:c r="A430">
-        <x:v>430</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="431">
-      <x:c r="A431">
-        <x:v>431</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="432">
-      <x:c r="A432">
-        <x:v>432</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="433">
-      <x:c r="A433">
-        <x:v>433</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="434">
-      <x:c r="A434">
-        <x:v>434</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="435">
-      <x:c r="A435">
-        <x:v>435</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="436">
-      <x:c r="A436">
-        <x:v>436</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="437">
-      <x:c r="A437">
-        <x:v>437</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="438">
-      <x:c r="A438">
-        <x:v>438</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="439">
-      <x:c r="A439">
-        <x:v>439</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="440">
-      <x:c r="A440">
-        <x:v>440</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="441">
-      <x:c r="A441">
-        <x:v>441</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="442">
-      <x:c r="A442">
-        <x:v>442</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="443">
-      <x:c r="A443">
-        <x:v>443</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="444">
-      <x:c r="A444">
-        <x:v>444</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="445">
-      <x:c r="A445">
-        <x:v>445</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="446">
-      <x:c r="A446">
-        <x:v>446</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="447">
-      <x:c r="A447">
-        <x:v>447</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="448">
-      <x:c r="A448">
-        <x:v>448</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="449">
-      <x:c r="A449">
-        <x:v>449</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="450">
-      <x:c r="A450">
-        <x:v>450</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="451">
-      <x:c r="A451">
-        <x:v>451</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="452">
-      <x:c r="A452">
-        <x:v>452</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="453">
-      <x:c r="A453">
-        <x:v>453</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="454">
-      <x:c r="A454">
-        <x:v>454</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="455">
-      <x:c r="A455">
-        <x:v>455</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="456">
-      <x:c r="A456">
-        <x:v>456</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="457">
-      <x:c r="A457">
-        <x:v>457</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="458">
-      <x:c r="A458">
-        <x:v>458</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="459">
-      <x:c r="A459">
-        <x:v>459</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="460">
-      <x:c r="A460">
-        <x:v>460</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="461">
-      <x:c r="A461">
-        <x:v>461</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="462">
-      <x:c r="A462">
-        <x:v>462</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="463">
-      <x:c r="A463">
-        <x:v>463</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="464">
-      <x:c r="A464">
-        <x:v>464</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="465">
-      <x:c r="A465">
-        <x:v>465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="466">
-      <x:c r="A466">
-        <x:v>466</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="467">
-      <x:c r="A467">
-        <x:v>467</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="468">
-      <x:c r="A468">
-        <x:v>468</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="469">
-      <x:c r="A469">
-        <x:v>469</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="470">
-      <x:c r="A470">
-        <x:v>470</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="471">
-      <x:c r="A471">
-        <x:v>471</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="472">
-      <x:c r="A472">
-        <x:v>472</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="473">
-      <x:c r="A473">
-        <x:v>473</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="474">
-      <x:c r="A474">
-        <x:v>474</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="475">
-      <x:c r="A475">
-        <x:v>475</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="476">
-      <x:c r="A476">
-        <x:v>476</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="477">
-      <x:c r="A477">
-        <x:v>477</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="478">
-      <x:c r="A478">
-        <x:v>478</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="479">
-      <x:c r="A479">
-        <x:v>479</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="480">
-      <x:c r="A480">
-        <x:v>480</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="481">
-      <x:c r="A481">
-        <x:v>481</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="482">
-      <x:c r="A482">
-        <x:v>482</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="483">
-      <x:c r="A483">
-        <x:v>483</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="484">
-      <x:c r="A484">
-        <x:v>484</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="485">
-      <x:c r="A485">
-        <x:v>485</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="486">
-      <x:c r="A486">
-        <x:v>486</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="487">
-      <x:c r="A487">
-        <x:v>487</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="488">
-      <x:c r="A488">
-        <x:v>488</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="489">
-      <x:c r="A489">
-        <x:v>489</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="490">
-      <x:c r="A490">
-        <x:v>490</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="491">
-      <x:c r="A491">
-        <x:v>491</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="492">
-      <x:c r="A492">
-        <x:v>492</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="493">
-      <x:c r="A493">
-        <x:v>493</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="494">
-      <x:c r="A494">
-        <x:v>494</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="495">
-      <x:c r="A495">
-        <x:v>495</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="496">
-      <x:c r="A496">
-        <x:v>496</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="497">
-      <x:c r="A497">
-        <x:v>497</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="498">
-      <x:c r="A498">
-        <x:v>498</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="499">
-      <x:c r="A499">
-        <x:v>499</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="500">
-      <x:c r="A500">
-        <x:v>500</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
no riesco a trovare una via d'scita per il printing delle celle in base al tempo
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK_PROVA_COLORE_2.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R487c925128044026"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rc65eb7eb034245a8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -1274,7 +1274,7 @@
     <x:t>COMMESSA</x:t>
   </x:si>
   <x:si>
-    <x:t>imnho</x:t>
+    <x:t>Ore Progetto</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1705,7 +1705,7 @@
 
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:NB6"/>
+  <x:dimension ref="A1:NB15"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -3288,11 +3288,41 @@
     </x:row>
     <x:row r="4">
       <x:c r="D4" t="s">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
     </x:row>
-    <x:row r="6">
-      <x:c r="A6" t="s">
+    <x:row r="9">
+      <x:c r="B9" t="s">
+        <x:v>420</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10">
+      <x:c r="B10" t="s">
+        <x:v>420</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11">
+      <x:c r="B11" t="s">
+        <x:v>420</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12">
+      <x:c r="B12" t="s">
+        <x:v>420</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13">
+      <x:c r="B13" t="s">
+        <x:v>420</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14">
+      <x:c r="B14" t="s">
+        <x:v>420</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15">
+      <x:c r="B15" t="s">
         <x:v>420</x:v>
       </x:c>
     </x:row>

</xml_diff>